<commit_message>
Frontend + Backend merged ✅✅✅✅
</commit_message>
<xml_diff>
--- a/backend/clientsPanels/public/SampleExcelSheet/Sample__Listing.xlsx
+++ b/backend/clientsPanels/public/SampleExcelSheet/Sample__Listing.xlsx
@@ -5,16 +5,16 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\Documents\Shadab-Builds\NMP-LATEST\mmapp\clientsPanels\public\SampleExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -633,6 +633,7 @@
     <col min="9" max="9" width="20.375" customWidth="1"/>
     <col min="10" max="10" width="22.5" customWidth="1"/>
     <col min="11" max="11" width="20.125" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Specification/ Accept Reject Done
</commit_message>
<xml_diff>
--- a/backend/clientsPanels/public/SampleExcelSheet/Sample__Listing.xlsx
+++ b/backend/clientsPanels/public/SampleExcelSheet/Sample__Listing.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\Documents\Shadab-Builds\NMP-LATEST\Web+Backend\backend\clientsPanels\public\SampleExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="4050" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Products" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Description</t>
   </si>
@@ -155,150 +155,7 @@
     <t>url must be end with extension (.png,.jpeg,.jpg) or use base64 image</t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>INDIA</t>
-  </si>
-  <si>
-    <t>Attributes</t>
-  </si>
-  <si>
-    <t>Specifications</t>
-  </si>
-  <si>
-    <t>45asa121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Copy the code below and paste it into any text/code editor. Fill in the details for each product variant you are listing in the bulk upload. The example provided includes details for 5 variants of a product.
-Feel free to customize the instructions based on your specific requirements or add any additional details you find necessary for your users.
-[
-    {
-        "attributes": {
-            "Size": "XL",
-            "Color": "red"
-        },
-        "sku": "SAMPLE-210",
-        "Mrp": "13.21",
-        "Selling Price": "10.12",
-        "Quantity": "10"
-    },
-    {
-        "attributes": {
-            "Size": "S",
-            "Color": "green"
-        },
-        "sku": "SAMPLE-211",
-        "Mrp": "9.99",
-        "Selling Price": "7.89",
-        "Quantity": "8"
-    },
-    {
-        "attributes": {
-            "Size": "M",
-            "Color": "blue"
-        },
-        "sku": "SAMPLE-212",
-        "Mrp": "11.45",
-        "Selling Price": "8.76",
-        "Quantity": "15"
-    },
-    {
-        "attributes": {
-            "Size": "L",
-            "Color": "yellow"
-        },
-        "sku": "SAMPLE-213",
-        "Mrp": "15.67",
-        "Selling Price": "12.34",
-        "Quantity": "5"
-    },
-    {
-        "attributes": {
-            "Size": "XXL",
-            "Color": "black"
-        },
-        "sku": "SAMPLE-214",
-        "Mrp": "17.89",
-        "Selling Price": "14.56",
-        "Quantity": "12"
-    }
-]
-</t>
-  </si>
-  <si>
-    <t>[
-    {
-        "attributes": {
-            "Size": "XL",
-            "Color": "red"
-        },
-        "sku": "SAMPLE-210",
-        "Mrp": "13.21",
-        "Selling Price": "10.12",
-        "Quantity": "10"
-    },
-    {
-        "attributes": {
-            "Size": "S",
-            "Color": "green"
-        },
-        "sku": "SAMPLE-211",
-        "Mrp": "9.99",
-        "Selling Price": "7.89",
-        "Quantity": "8"
-    },
-    {
-        "attributes": {
-            "Size": "M",
-            "Color": "blue"
-        },
-        "sku": "SAMPLE-212",
-        "Mrp": "11.45",
-        "Selling Price": "8.76",
-        "Quantity": "15"
-    },
-    {
-        "attributes": {
-            "Size": "L",
-            "Color": "yellow"
-        },
-        "sku": "SAMPLE-213",
-        "Mrp": "15.67",
-        "Selling Price": "12.34",
-        "Quantity": "5"
-    },
-    {
-        "attributes": {
-            "Size": "XXL",
-            "Color": "black"
-        },
-        "sku": "SAMPLE-214",
-        "Mrp": "17.89",
-        "Selling Price": "14.56",
-        "Quantity": "12"
-    }
-]</t>
-  </si>
-  <si>
-    <t>Variant</t>
-  </si>
-  <si>
     <t>if there is attribute then type Variant else type Simple</t>
-  </si>
-  <si>
-    <t>{
-  "Warranty": "Yes, 1 year warranty",
-  "Material": "Cotton",
-  "Fit": "Regular Fit",
-  "Pattern": "Solid",
-  "Sleeve Length": "Full Sleeves",
-  "Collar Type": "Button-Down Collar",
-  "Occasion": "Casual",
-  "Color": "Red",
-  "Brand": "XYZ Brand",
-  "Price": "$29.99"
-}</t>
   </si>
 </sst>
 </file>
@@ -405,7 +262,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -416,12 +273,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -781,34 +632,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z7"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="37.375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="5" max="5" width="26.125" customWidth="1"/>
-    <col min="6" max="6" width="21.875" customWidth="1"/>
-    <col min="7" max="7" width="28.5" customWidth="1"/>
-    <col min="8" max="8" width="22.625" customWidth="1"/>
-    <col min="9" max="9" width="20.375" customWidth="1"/>
-    <col min="10" max="10" width="22.5" customWidth="1"/>
-    <col min="11" max="11" width="20.125" customWidth="1"/>
-    <col min="12" max="12" width="15.25" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="24" customWidth="1"/>
-    <col min="15" max="15" width="49.125" customWidth="1"/>
-    <col min="20" max="20" width="10.625" customWidth="1"/>
-    <col min="24" max="24" width="20.75" customWidth="1"/>
+    <col min="1" max="1" width="45.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="88.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="76.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="79.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
@@ -878,14 +737,8 @@
       <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="2" spans="1:26" s="5" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>15</v>
       </c>
@@ -934,14 +787,8 @@
       <c r="X2" s="5">
         <v>10</v>
       </c>
-      <c r="Y2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
@@ -976,80 +823,27 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5">
-        <v>452</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="7">
-        <v>102</v>
-      </c>
-      <c r="R5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S5">
-        <v>10</v>
-      </c>
-      <c r="T5" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5">
-        <v>45</v>
-      </c>
-      <c r="V5">
-        <v>44</v>
-      </c>
-      <c r="W5">
-        <v>54</v>
-      </c>
-      <c r="X5">
-        <v>4</v>
-      </c>
-      <c r="Y5" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>52</v>
-      </c>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:26" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="G7" s="7"/>

</xml_diff>